<commit_message>
Excel file reading and writing
</commit_message>
<xml_diff>
--- a/src/com/syntax/class35/Test.xlsx
+++ b/src/com/syntax/class35/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asghar Nazir\IdeaProjects\JavaBatch8\src\com\syntax\class35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E74316-6E61-478D-91BE-72BF26E2BCDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682ED025-1B3E-49B1-A589-8680B2778250}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41595" yWindow="3915" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstPage" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>First Name</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Age</t>
+  </si>
+  <si>
+    <t>age</t>
   </si>
 </sst>
 </file>
@@ -395,21 +398,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="26.5546875" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,8 +428,17 @@
       <c r="D1" t="s">
         <v>16</v>
       </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -437,7 +452,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -451,7 +466,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -465,7 +480,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>

</xml_diff>